<commit_message>
added overdose control for sensitivity analysis
</commit_message>
<xml_diff>
--- a/Data/CleanData/StateRandomEffects.xlsx
+++ b/Data/CleanData/StateRandomEffects.xlsx
@@ -380,7 +380,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>-0.2107096300663047</v>
+        <v>-0.2107326532823305</v>
       </c>
     </row>
     <row r="3">
@@ -390,7 +390,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>-0.3285805487383965</v>
+        <v>-0.3285089167286134</v>
       </c>
     </row>
     <row r="4">
@@ -400,7 +400,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.8626092557968615</v>
+        <v>0.8626238570950225</v>
       </c>
     </row>
     <row r="5">
@@ -410,7 +410,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>-0.5567967572394513</v>
+        <v>-0.5567702826317268</v>
       </c>
     </row>
     <row r="6">
@@ -420,7 +420,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>-1.117523565389231</v>
+        <v>-1.117332931268181</v>
       </c>
     </row>
     <row r="7">
@@ -430,7 +430,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>1.183302178448496</v>
+        <v>1.183351418893715</v>
       </c>
     </row>
     <row r="8">
@@ -440,7 +440,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>-1.115999566352717</v>
+        <v>-1.11604088344161</v>
       </c>
     </row>
     <row r="9">
@@ -450,7 +450,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>-0.8431620289226631</v>
+        <v>-0.8432506092089281</v>
       </c>
     </row>
     <row r="10">
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>-1.552853273901155</v>
+        <v>-1.552975796082729</v>
       </c>
     </row>
     <row r="11">
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.3794926309675766</v>
+        <v>0.3795097030527969</v>
       </c>
     </row>
     <row r="12">
@@ -480,7 +480,7 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.7660564712056283</v>
+        <v>0.7660564747966165</v>
       </c>
     </row>
     <row r="13">
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="B13">
-        <v>-0.08597802141424034</v>
+        <v>-0.08596922480107251</v>
       </c>
     </row>
     <row r="14">
@@ -500,7 +500,7 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.9691686055704397</v>
+        <v>0.9691932892602967</v>
       </c>
     </row>
     <row r="15">
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.7868800587357219</v>
+        <v>0.7869228202624792</v>
       </c>
     </row>
     <row r="16">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="B16">
-        <v>0.523488094696101</v>
+        <v>0.5235084108411926</v>
       </c>
     </row>
     <row r="17">
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="B17">
-        <v>-0.5612322195000994</v>
+        <v>-0.5611821251704674</v>
       </c>
     </row>
     <row r="18">
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.2968937320605084</v>
+        <v>0.296888637459287</v>
       </c>
     </row>
     <row r="19">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="B19">
-        <v>1.213808316179295</v>
+        <v>1.213865710618471</v>
       </c>
     </row>
     <row r="20">
@@ -560,7 +560,7 @@
         </is>
       </c>
       <c r="B20">
-        <v>0.4854471346242175</v>
+        <v>0.4854550930935883</v>
       </c>
     </row>
     <row r="21">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="B21">
-        <v>0.9145510847677037</v>
+        <v>0.9145218025375009</v>
       </c>
     </row>
     <row r="22">
@@ -580,7 +580,7 @@
         </is>
       </c>
       <c r="B22">
-        <v>1.162128347750292</v>
+        <v>1.162077842411568</v>
       </c>
     </row>
     <row r="23">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.08499270357886061</v>
+        <v>0.08494002554866097</v>
       </c>
     </row>
     <row r="24">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.5665803266537462</v>
+        <v>0.566637787777987</v>
       </c>
     </row>
     <row r="25">
@@ -610,7 +610,7 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.8800417775141355</v>
+        <v>0.8800893255643465</v>
       </c>
     </row>
     <row r="26">
@@ -620,7 +620,7 @@
         </is>
       </c>
       <c r="B26">
-        <v>-0.4572652922786732</v>
+        <v>-0.4573060797737802</v>
       </c>
     </row>
     <row r="27">
@@ -630,7 +630,7 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.006859567148981245</v>
+        <v>0.006862388379346735</v>
       </c>
     </row>
     <row r="28">
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="B28">
-        <v>-0.6689488367979073</v>
+        <v>-0.6689075631707138</v>
       </c>
     </row>
     <row r="29">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="B29">
-        <v>-0.4553647393943374</v>
+        <v>-0.455391379997536</v>
       </c>
     </row>
     <row r="30">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="B30">
-        <v>-0.2838598611087938</v>
+        <v>-0.2838724847735811</v>
       </c>
     </row>
     <row r="31">
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="B31">
-        <v>-0.4871918559230149</v>
+        <v>-0.4872098142395328</v>
       </c>
     </row>
     <row r="32">
@@ -680,7 +680,7 @@
         </is>
       </c>
       <c r="B32">
-        <v>0.5622937104604721</v>
+        <v>0.5622308029564578</v>
       </c>
     </row>
     <row r="33">
@@ -690,7 +690,7 @@
         </is>
       </c>
       <c r="B33">
-        <v>0.506367630133558</v>
+        <v>0.5063278499450848</v>
       </c>
     </row>
     <row r="34">
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="B34">
-        <v>-0.4878818198784703</v>
+        <v>-0.4878658938491042</v>
       </c>
     </row>
     <row r="35">
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="B35">
-        <v>1.065249799183251</v>
+        <v>1.065256617684329</v>
       </c>
     </row>
     <row r="36">
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="B36">
-        <v>0.07717723264610546</v>
+        <v>0.07722228031321896</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="B37">
-        <v>-0.4142333487413991</v>
+        <v>-0.4141713454091082</v>
       </c>
     </row>
     <row r="38">
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.2246042860006618</v>
+        <v>0.2245907131098721</v>
       </c>
     </row>
     <row r="39">
@@ -750,7 +750,7 @@
         </is>
       </c>
       <c r="B39">
-        <v>0.2471326585944414</v>
+        <v>0.2471596654245625</v>
       </c>
     </row>
     <row r="40">
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="B40">
-        <v>0.4930437594810862</v>
+        <v>0.4930834592983986</v>
       </c>
     </row>
     <row r="41">
@@ -770,7 +770,7 @@
         </is>
       </c>
       <c r="B41">
-        <v>-1.033410100280771</v>
+        <v>-1.033491399908844</v>
       </c>
     </row>
     <row r="42">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="B42">
-        <v>-0.478316911800977</v>
+        <v>-0.4783282906657406</v>
       </c>
     </row>
     <row r="43">
@@ -790,7 +790,7 @@
         </is>
       </c>
       <c r="B43">
-        <v>-1.035912555809179</v>
+        <v>-1.035932860804692</v>
       </c>
     </row>
     <row r="44">
@@ -800,7 +800,7 @@
         </is>
       </c>
       <c r="B44">
-        <v>0.1928526531182913</v>
+        <v>0.1928727562928887</v>
       </c>
     </row>
     <row r="45">
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="B45">
-        <v>-0.7195718048211917</v>
+        <v>-0.7195048374358026</v>
       </c>
     </row>
     <row r="46">
@@ -820,7 +820,7 @@
         </is>
       </c>
       <c r="B46">
-        <v>0.981367213570524</v>
+        <v>0.9814045632970432</v>
       </c>
     </row>
     <row r="47">
@@ -830,7 +830,7 @@
         </is>
       </c>
       <c r="B47">
-        <v>-1.761740799382168</v>
+        <v>-1.761734223143563</v>
       </c>
     </row>
     <row r="48">
@@ -840,7 +840,7 @@
         </is>
       </c>
       <c r="B48">
-        <v>-0.1257070197089596</v>
+        <v>-0.1257026993871829</v>
       </c>
     </row>
     <row r="49">
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="B49">
-        <v>0.8419302401053328</v>
+        <v>0.8420100714767016</v>
       </c>
     </row>
     <row r="50">
@@ -860,7 +860,7 @@
         </is>
       </c>
       <c r="B50">
-        <v>-0.6481010370827559</v>
+        <v>-0.6480714110313354</v>
       </c>
     </row>
     <row r="51">
@@ -870,7 +870,7 @@
         </is>
       </c>
       <c r="B51">
-        <v>0.4734040413373887</v>
+        <v>0.4734487870484301</v>
       </c>
     </row>
     <row r="52">
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="B52">
-        <v>-1.181768699621209</v>
+        <v>-1.181753096155747</v>
       </c>
     </row>
   </sheetData>
@@ -915,7 +915,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>-0.1695175496852171</v>
+        <v>-0.1693193676389557</v>
       </c>
     </row>
     <row r="3">
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>-0.2222181934628645</v>
+        <v>-0.221258738098225</v>
       </c>
     </row>
     <row r="4">
@@ -935,7 +935,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.653328510049679</v>
+        <v>0.6541278080871633</v>
       </c>
     </row>
     <row r="5">
@@ -945,7 +945,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>0.2162570096603093</v>
+        <v>0.2167936097345974</v>
       </c>
     </row>
     <row r="6">
@@ -955,7 +955,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>-0.1848971421706865</v>
+        <v>-0.184778668832089</v>
       </c>
     </row>
     <row r="7">
@@ -965,7 +965,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.6253208964046587</v>
+        <v>0.6260223068331543</v>
       </c>
     </row>
     <row r="8">
@@ -975,7 +975,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.7732870878610397</v>
+        <v>0.7736869647904464</v>
       </c>
     </row>
     <row r="9">
@@ -985,7 +985,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>-1.161533488466614</v>
+        <v>-1.161309031842669</v>
       </c>
     </row>
     <row r="10">
@@ -995,7 +995,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>-1.319792966862148</v>
+        <v>-1.32034984627818</v>
       </c>
     </row>
     <row r="11">
@@ -1005,7 +1005,7 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.01455118467319229</v>
+        <v>0.01489364812551331</v>
       </c>
     </row>
     <row r="12">
@@ -1015,7 +1015,7 @@
         </is>
       </c>
       <c r="B12">
-        <v>-0.5668689407237995</v>
+        <v>-0.5668264315376936</v>
       </c>
     </row>
     <row r="13">
@@ -1025,7 +1025,7 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.7824550971442956</v>
+        <v>0.7823505612690713</v>
       </c>
     </row>
     <row r="14">
@@ -1035,7 +1035,7 @@
         </is>
       </c>
       <c r="B14">
-        <v>-1.55549496684002</v>
+        <v>-1.554439630692183</v>
       </c>
     </row>
     <row r="15">
@@ -1045,7 +1045,7 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.8892840879685002</v>
+        <v>0.889625582256208</v>
       </c>
     </row>
     <row r="16">
@@ -1055,7 +1055,7 @@
         </is>
       </c>
       <c r="B16">
-        <v>0.6086614245791945</v>
+        <v>0.6091990020524504</v>
       </c>
     </row>
     <row r="17">
@@ -1065,7 +1065,7 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.6007617578596708</v>
+        <v>0.6015464471938033</v>
       </c>
     </row>
     <row r="18">
@@ -1075,7 +1075,7 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.2582801590122458</v>
+        <v>0.2590759701860573</v>
       </c>
     </row>
     <row r="19">
@@ -1085,7 +1085,7 @@
         </is>
       </c>
       <c r="B19">
-        <v>0.8608567444383043</v>
+        <v>0.8614730259207737</v>
       </c>
     </row>
     <row r="20">
@@ -1095,7 +1095,7 @@
         </is>
       </c>
       <c r="B20">
-        <v>-0.7158329774234646</v>
+        <v>-0.715674738110565</v>
       </c>
     </row>
     <row r="21">
@@ -1105,7 +1105,7 @@
         </is>
       </c>
       <c r="B21">
-        <v>0.1730345095767379</v>
+        <v>0.1736367345547335</v>
       </c>
     </row>
     <row r="22">
@@ -1115,7 +1115,7 @@
         </is>
       </c>
       <c r="B22">
-        <v>0.2316367538777333</v>
+        <v>0.2315727400495358</v>
       </c>
     </row>
     <row r="23">
@@ -1125,7 +1125,7 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.8927563695169739</v>
+        <v>0.892973869840605</v>
       </c>
     </row>
     <row r="24">
@@ -1135,7 +1135,7 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.6668616651813118</v>
+        <v>0.6671970054292965</v>
       </c>
     </row>
     <row r="25">
@@ -1145,7 +1145,7 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.6105811503632724</v>
+        <v>0.6112430370159492</v>
       </c>
     </row>
     <row r="26">
@@ -1155,7 +1155,7 @@
         </is>
       </c>
       <c r="B26">
-        <v>-0.5574259748895422</v>
+        <v>-0.5573113811559901</v>
       </c>
     </row>
     <row r="27">
@@ -1165,7 +1165,7 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.6529964460021935</v>
+        <v>0.6534530988280282</v>
       </c>
     </row>
     <row r="28">
@@ -1175,7 +1175,7 @@
         </is>
       </c>
       <c r="B28">
-        <v>-0.4916521491586364</v>
+        <v>-0.4908425707899471</v>
       </c>
     </row>
     <row r="29">
@@ -1185,7 +1185,7 @@
         </is>
       </c>
       <c r="B29">
-        <v>0.1329313817510104</v>
+        <v>0.1337543727706917</v>
       </c>
     </row>
     <row r="30">
@@ -1195,7 +1195,7 @@
         </is>
       </c>
       <c r="B30">
-        <v>-0.5341319504163035</v>
+        <v>-0.5332636949767861</v>
       </c>
     </row>
     <row r="31">
@@ -1205,7 +1205,7 @@
         </is>
       </c>
       <c r="B31">
-        <v>-0.7291918356475732</v>
+        <v>-0.7285725145158102</v>
       </c>
     </row>
     <row r="32">
@@ -1215,7 +1215,7 @@
         </is>
       </c>
       <c r="B32">
-        <v>0.390212056931589</v>
+        <v>0.3905794781572773</v>
       </c>
     </row>
     <row r="33">
@@ -1225,7 +1225,7 @@
         </is>
       </c>
       <c r="B33">
-        <v>0.05089073959906423</v>
+        <v>0.051915315694388</v>
       </c>
     </row>
     <row r="34">
@@ -1235,7 +1235,7 @@
         </is>
       </c>
       <c r="B34">
-        <v>0.8836500175751054</v>
+        <v>0.8836475993565989</v>
       </c>
     </row>
     <row r="35">
@@ -1245,7 +1245,7 @@
         </is>
       </c>
       <c r="B35">
-        <v>0.2846845287788118</v>
+        <v>0.284861343224673</v>
       </c>
     </row>
     <row r="36">
@@ -1255,7 +1255,7 @@
         </is>
       </c>
       <c r="B36">
-        <v>-1.067881041730398</v>
+        <v>-1.066754424716891</v>
       </c>
     </row>
     <row r="37">
@@ -1265,7 +1265,7 @@
         </is>
       </c>
       <c r="B37">
-        <v>0.8280519601031143</v>
+        <v>0.8283593738336013</v>
       </c>
     </row>
     <row r="38">
@@ -1275,7 +1275,7 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.1456659546845397</v>
+        <v>0.1462103210071088</v>
       </c>
     </row>
     <row r="39">
@@ -1285,7 +1285,7 @@
         </is>
       </c>
       <c r="B39">
-        <v>0.3993001077312155</v>
+        <v>0.3998274485635739</v>
       </c>
     </row>
     <row r="40">
@@ -1295,7 +1295,7 @@
         </is>
       </c>
       <c r="B40">
-        <v>0.6592785062088932</v>
+        <v>0.6595979467188182</v>
       </c>
     </row>
     <row r="41">
@@ -1305,7 +1305,7 @@
         </is>
       </c>
       <c r="B41">
-        <v>-0.7278781221028975</v>
+        <v>-0.7274778030566553</v>
       </c>
     </row>
     <row r="42">
@@ -1315,7 +1315,7 @@
         </is>
       </c>
       <c r="B42">
-        <v>-0.9070795660533716</v>
+        <v>-0.9069177070273359</v>
       </c>
     </row>
     <row r="43">
@@ -1325,7 +1325,7 @@
         </is>
       </c>
       <c r="B43">
-        <v>-0.6643985931450389</v>
+        <v>-0.6635114185639509</v>
       </c>
     </row>
     <row r="44">
@@ -1335,7 +1335,7 @@
         </is>
       </c>
       <c r="B44">
-        <v>0.3711187768032389</v>
+        <v>0.3714712449322368</v>
       </c>
     </row>
     <row r="45">
@@ -1345,7 +1345,7 @@
         </is>
       </c>
       <c r="B45">
-        <v>-0.8972086450442145</v>
+        <v>-0.8966419594099232</v>
       </c>
     </row>
     <row r="46">
@@ -1355,7 +1355,7 @@
         </is>
       </c>
       <c r="B46">
-        <v>-0.1644564990618951</v>
+        <v>-0.1634361948990848</v>
       </c>
     </row>
     <row r="47">
@@ -1365,7 +1365,7 @@
         </is>
       </c>
       <c r="B47">
-        <v>-0.5659264718363847</v>
+        <v>-0.5653844387089546</v>
       </c>
     </row>
     <row r="48">
@@ -1375,7 +1375,7 @@
         </is>
       </c>
       <c r="B48">
-        <v>-0.8170496131347321</v>
+        <v>-0.8167676718071686</v>
       </c>
     </row>
     <row r="49">
@@ -1385,7 +1385,7 @@
         </is>
       </c>
       <c r="B49">
-        <v>0.6075191316218623</v>
+        <v>0.6080610976246914</v>
       </c>
     </row>
     <row r="50">
@@ -1395,7 +1395,7 @@
         </is>
       </c>
       <c r="B50">
-        <v>0.1529810290138089</v>
+        <v>0.1538073161694786</v>
       </c>
     </row>
     <row r="51">
@@ -1405,7 +1405,7 @@
         </is>
       </c>
       <c r="B51">
-        <v>0.2677114387654328</v>
+        <v>0.2683362390492197</v>
       </c>
     </row>
     <row r="52">
@@ -1415,7 +1415,7 @@
         </is>
       </c>
       <c r="B52">
-        <v>-0.5973483075860188</v>
+        <v>-0.59612692302143</v>
       </c>
     </row>
   </sheetData>
@@ -1450,7 +1450,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>-0.08108460132415919</v>
+        <v>-0.08052430516249021</v>
       </c>
     </row>
     <row r="3">
@@ -1460,7 +1460,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>-0.001742240811412345</v>
+        <v>8.38897759084388E-05</v>
       </c>
     </row>
     <row r="4">
@@ -1470,7 +1470,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.2768029718096486</v>
+        <v>0.2772329702369824</v>
       </c>
     </row>
     <row r="5">
@@ -1480,7 +1480,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>-0.7748328378808831</v>
+        <v>-0.7743402444207682</v>
       </c>
     </row>
     <row r="6">
@@ -1490,7 +1490,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>-0.7151345219911827</v>
+        <v>-0.7148687644027398</v>
       </c>
     </row>
     <row r="7">
@@ -1500,7 +1500,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.05854339432051642</v>
+        <v>0.05902901130349057</v>
       </c>
     </row>
     <row r="8">
@@ -1510,7 +1510,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.189179946740731</v>
+        <v>0.1885960941099055</v>
       </c>
     </row>
     <row r="9">
@@ -1520,7 +1520,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>-1.519099084724192</v>
+        <v>-1.519294377745518</v>
       </c>
     </row>
     <row r="10">
@@ -1530,7 +1530,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>-1.338682609055229</v>
+        <v>-1.339763990857971</v>
       </c>
     </row>
     <row r="11">
@@ -1540,7 +1540,7 @@
         </is>
       </c>
       <c r="B11">
-        <v>-0.6659244183420761</v>
+        <v>-0.6658244192043324</v>
       </c>
     </row>
     <row r="12">
@@ -1550,7 +1550,7 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.8008471132227915</v>
+        <v>0.8014842078003478</v>
       </c>
     </row>
     <row r="13">
@@ -1560,7 +1560,7 @@
         </is>
       </c>
       <c r="B13">
-        <v>-1.325354520439601</v>
+        <v>-1.322635601011907</v>
       </c>
     </row>
     <row r="14">
@@ -1570,7 +1570,7 @@
         </is>
       </c>
       <c r="B14">
-        <v>-0.1008509340782001</v>
+        <v>-0.099980202326338</v>
       </c>
     </row>
     <row r="15">
@@ -1580,7 +1580,7 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.01635656530065821</v>
+        <v>0.01654093906740731</v>
       </c>
     </row>
     <row r="16">
@@ -1590,7 +1590,7 @@
         </is>
       </c>
       <c r="B16">
-        <v>-0.383059343662972</v>
+        <v>-0.3827834487002213</v>
       </c>
     </row>
     <row r="17">
@@ -1600,7 +1600,7 @@
         </is>
       </c>
       <c r="B17">
-        <v>-0.4058869669265243</v>
+        <v>-0.4054127493802704</v>
       </c>
     </row>
     <row r="18">
@@ -1610,7 +1610,7 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.6250417932104905</v>
+        <v>0.6258901529127305</v>
       </c>
     </row>
     <row r="19">
@@ -1620,7 +1620,7 @@
         </is>
       </c>
       <c r="B19">
-        <v>-0.6447373117067832</v>
+        <v>-0.6443361590093264</v>
       </c>
     </row>
     <row r="20">
@@ -1630,7 +1630,7 @@
         </is>
       </c>
       <c r="B20">
-        <v>0.908533979818997</v>
+        <v>0.9090221850191205</v>
       </c>
     </row>
     <row r="21">
@@ -1640,7 +1640,7 @@
         </is>
       </c>
       <c r="B21">
-        <v>-0.09616480938771775</v>
+        <v>-0.09636425964788412</v>
       </c>
     </row>
     <row r="22">
@@ -1650,7 +1650,7 @@
         </is>
       </c>
       <c r="B22">
-        <v>1.145267821326315</v>
+        <v>1.145441762336221</v>
       </c>
     </row>
     <row r="23">
@@ -1660,7 +1660,7 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.1130276854167859</v>
+        <v>0.1123345316256893</v>
       </c>
     </row>
     <row r="24">
@@ -1670,7 +1670,7 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.9495624392872207</v>
+        <v>0.9500224040172693</v>
       </c>
     </row>
     <row r="25">
@@ -1680,7 +1680,7 @@
         </is>
       </c>
       <c r="B25">
-        <v>1.045435267274211</v>
+        <v>1.046011821030861</v>
       </c>
     </row>
     <row r="26">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="B26">
-        <v>0.6063989905054424</v>
+        <v>0.6071613831168229</v>
       </c>
     </row>
     <row r="27">
@@ -1700,7 +1700,7 @@
         </is>
       </c>
       <c r="B27">
-        <v>-0.3381124835335337</v>
+        <v>-0.3378632060941346</v>
       </c>
     </row>
     <row r="28">
@@ -1710,7 +1710,7 @@
         </is>
       </c>
       <c r="B28">
-        <v>0.1603559275861986</v>
+        <v>0.1609906495855439</v>
       </c>
     </row>
     <row r="29">
@@ -1720,7 +1720,7 @@
         </is>
       </c>
       <c r="B29">
-        <v>0.5129763907551531</v>
+        <v>0.5135818556552071</v>
       </c>
     </row>
     <row r="30">
@@ -1730,7 +1730,7 @@
         </is>
       </c>
       <c r="B30">
-        <v>-0.520275080862278</v>
+        <v>-0.5189931991410623</v>
       </c>
     </row>
     <row r="31">
@@ -1740,7 +1740,7 @@
         </is>
       </c>
       <c r="B31">
-        <v>-1.817373075827484</v>
+        <v>-1.817570364420324</v>
       </c>
     </row>
     <row r="32">
@@ -1750,7 +1750,7 @@
         </is>
       </c>
       <c r="B32">
-        <v>-0.03176435963002326</v>
+        <v>-0.03162857461862049</v>
       </c>
     </row>
     <row r="33">
@@ -1760,7 +1760,7 @@
         </is>
       </c>
       <c r="B33">
-        <v>0.6969433915405137</v>
+        <v>0.6970216174240549</v>
       </c>
     </row>
     <row r="34">
@@ -1770,7 +1770,7 @@
         </is>
       </c>
       <c r="B34">
-        <v>0.9770345967824766</v>
+        <v>0.9766506366266791</v>
       </c>
     </row>
     <row r="35">
@@ -1780,7 +1780,7 @@
         </is>
       </c>
       <c r="B35">
-        <v>0.3624579894666846</v>
+        <v>0.3629004436065341</v>
       </c>
     </row>
     <row r="36">
@@ -1790,7 +1790,7 @@
         </is>
       </c>
       <c r="B36">
-        <v>0.093398188376644</v>
+        <v>0.09494033231427727</v>
       </c>
     </row>
     <row r="37">
@@ -1800,7 +1800,7 @@
         </is>
       </c>
       <c r="B37">
-        <v>0.2719570392224911</v>
+        <v>0.2719948792944492</v>
       </c>
     </row>
     <row r="38">
@@ -1810,7 +1810,7 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.9693715148120021</v>
+        <v>0.9700139501012744</v>
       </c>
     </row>
     <row r="39">
@@ -1820,7 +1820,7 @@
         </is>
       </c>
       <c r="B39">
-        <v>0.8780827567853325</v>
+        <v>0.8780532986105821</v>
       </c>
     </row>
     <row r="40">
@@ -1830,7 +1830,7 @@
         </is>
       </c>
       <c r="B40">
-        <v>-0.7527965231078599</v>
+        <v>-0.7528404639440259</v>
       </c>
     </row>
     <row r="41">
@@ -1840,7 +1840,7 @@
         </is>
       </c>
       <c r="B41">
-        <v>-0.9996755437711566</v>
+        <v>-1.000157506213422</v>
       </c>
     </row>
     <row r="42">
@@ -1850,7 +1850,7 @@
         </is>
       </c>
       <c r="B42">
-        <v>0.9436093807949301</v>
+        <v>0.9439845472270046</v>
       </c>
     </row>
     <row r="43">
@@ -1860,7 +1860,7 @@
         </is>
       </c>
       <c r="B43">
-        <v>0.2878917748667326</v>
+        <v>0.2887426042905565</v>
       </c>
     </row>
     <row r="44">
@@ -1870,7 +1870,7 @@
         </is>
       </c>
       <c r="B44">
-        <v>-1.092176983400562</v>
+        <v>-1.091923303097379</v>
       </c>
     </row>
     <row r="45">
@@ -1880,7 +1880,7 @@
         </is>
       </c>
       <c r="B45">
-        <v>-1.147967674508756</v>
+        <v>-1.147621739947163</v>
       </c>
     </row>
     <row r="46">
@@ -1890,7 +1890,7 @@
         </is>
       </c>
       <c r="B46">
-        <v>0.5756421516157544</v>
+        <v>0.5768793844482697</v>
       </c>
     </row>
     <row r="47">
@@ -1900,7 +1900,7 @@
         </is>
       </c>
       <c r="B47">
-        <v>-1.390155986736243</v>
+        <v>-1.390630204353133</v>
       </c>
     </row>
     <row r="48">
@@ -1910,7 +1910,7 @@
         </is>
       </c>
       <c r="B48">
-        <v>1.501961456250036</v>
+        <v>1.502668955877126</v>
       </c>
     </row>
     <row r="49">
@@ -1920,7 +1920,7 @@
         </is>
       </c>
       <c r="B49">
-        <v>1.082816743681575</v>
+        <v>1.083485450638274</v>
       </c>
     </row>
     <row r="50">
@@ -1930,7 +1930,7 @@
         </is>
       </c>
       <c r="B50">
-        <v>-0.3961913442196406</v>
+        <v>-0.3958691021105883</v>
       </c>
     </row>
     <row r="51">
@@ -1940,7 +1940,7 @@
         </is>
       </c>
       <c r="B51">
-        <v>1.212004862982891</v>
+        <v>1.212431872265201</v>
       </c>
     </row>
     <row r="52">
@@ -1950,7 +1950,7 @@
         </is>
       </c>
       <c r="B52">
-        <v>-0.287122638289798</v>
+        <v>-0.2858026104857197</v>
       </c>
     </row>
   </sheetData>
@@ -1985,7 +1985,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>-0.3020155664608553</v>
+        <v>-0.3019866373008651</v>
       </c>
     </row>
     <row r="3">
@@ -1995,7 +1995,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>-0.05117455808853861</v>
+        <v>-0.05103854888699403</v>
       </c>
     </row>
     <row r="4">
@@ -2005,7 +2005,7 @@
         </is>
       </c>
       <c r="B4">
-        <v>0.6310724272858534</v>
+        <v>0.6310530559667228</v>
       </c>
     </row>
     <row r="5">
@@ -2015,7 +2015,7 @@
         </is>
       </c>
       <c r="B5">
-        <v>-0.1579592759084945</v>
+        <v>-0.1579557983582583</v>
       </c>
     </row>
     <row r="6">
@@ -2025,7 +2025,7 @@
         </is>
       </c>
       <c r="B6">
-        <v>-0.7268839675391212</v>
+        <v>-0.7267822032957377</v>
       </c>
     </row>
     <row r="7">
@@ -2035,7 +2035,7 @@
         </is>
       </c>
       <c r="B7">
-        <v>0.7349134033300365</v>
+        <v>0.7348930505083187</v>
       </c>
     </row>
     <row r="8">
@@ -2045,7 +2045,7 @@
         </is>
       </c>
       <c r="B8">
-        <v>0.2996678411792817</v>
+        <v>0.2996367603965951</v>
       </c>
     </row>
     <row r="9">
@@ -2055,7 +2055,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>-1.139311714324985</v>
+        <v>-1.139305797550153</v>
       </c>
     </row>
     <row r="10">
@@ -2065,7 +2065,7 @@
         </is>
       </c>
       <c r="B10">
-        <v>-1.383185946063802</v>
+        <v>-1.383089473562751</v>
       </c>
     </row>
     <row r="11">
@@ -2075,7 +2075,7 @@
         </is>
       </c>
       <c r="B11">
-        <v>0.04671982713181191</v>
+        <v>0.04674265139039078</v>
       </c>
     </row>
     <row r="12">
@@ -2085,7 +2085,7 @@
         </is>
       </c>
       <c r="B12">
-        <v>0.09356018428129514</v>
+        <v>0.09363775263897317</v>
       </c>
     </row>
     <row r="13">
@@ -2095,7 +2095,7 @@
         </is>
       </c>
       <c r="B13">
-        <v>0.2769068821245325</v>
+        <v>0.277147421522158</v>
       </c>
     </row>
     <row r="14">
@@ -2105,7 +2105,7 @@
         </is>
       </c>
       <c r="B14">
-        <v>-0.0333722829406122</v>
+        <v>-0.03341395504256857</v>
       </c>
     </row>
     <row r="15">
@@ -2115,7 +2115,7 @@
         </is>
       </c>
       <c r="B15">
-        <v>0.6654125039776517</v>
+        <v>0.6654307875349142</v>
       </c>
     </row>
     <row r="16">
@@ -2125,7 +2125,7 @@
         </is>
       </c>
       <c r="B16">
-        <v>0.4029436908643569</v>
+        <v>0.4029260464877222</v>
       </c>
     </row>
     <row r="17">
@@ -2135,7 +2135,7 @@
         </is>
       </c>
       <c r="B17">
-        <v>0.06604062630455311</v>
+        <v>0.06600286887826992</v>
       </c>
     </row>
     <row r="18">
@@ -2145,7 +2145,7 @@
         </is>
       </c>
       <c r="B18">
-        <v>0.2054379455306424</v>
+        <v>0.2054114404958935</v>
       </c>
     </row>
     <row r="19">
@@ -2155,7 +2155,7 @@
         </is>
       </c>
       <c r="B19">
-        <v>0.8026895054318718</v>
+        <v>0.8026651320446875</v>
       </c>
     </row>
     <row r="20">
@@ -2165,7 +2165,7 @@
         </is>
       </c>
       <c r="B20">
-        <v>-0.08180422970961104</v>
+        <v>-0.08173143486957839</v>
       </c>
     </row>
     <row r="21">
@@ -2175,7 +2175,7 @@
         </is>
       </c>
       <c r="B21">
-        <v>0.406945892534713</v>
+        <v>0.4068774618731519</v>
       </c>
     </row>
     <row r="22">
@@ -2185,7 +2185,7 @@
         </is>
       </c>
       <c r="B22">
-        <v>0.6256512355291427</v>
+        <v>0.6257066645208705</v>
       </c>
     </row>
     <row r="23">
@@ -2195,7 +2195,7 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.513599965829839</v>
+        <v>0.5135632486058881</v>
       </c>
     </row>
     <row r="24">
@@ -2205,7 +2205,7 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.5077498607958199</v>
+        <v>0.5077635258330078</v>
       </c>
     </row>
     <row r="25">
@@ -2215,7 +2215,7 @@
         </is>
       </c>
       <c r="B25">
-        <v>0.6352508032987695</v>
+        <v>0.6352388679954268</v>
       </c>
     </row>
     <row r="26">
@@ -2225,7 +2225,7 @@
         </is>
       </c>
       <c r="B26">
-        <v>-0.3977753829373302</v>
+        <v>-0.3977028980126575</v>
       </c>
     </row>
     <row r="27">
@@ -2235,7 +2235,7 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.2848382100113157</v>
+        <v>0.2848261746449285</v>
       </c>
     </row>
     <row r="28">
@@ -2245,7 +2245,7 @@
         </is>
       </c>
       <c r="B28">
-        <v>-0.5030986966213974</v>
+        <v>-0.5031087316277191</v>
       </c>
     </row>
     <row r="29">
@@ -2255,7 +2255,7 @@
         </is>
       </c>
       <c r="B29">
-        <v>-0.07609532274231182</v>
+        <v>-0.07613314752392485</v>
       </c>
     </row>
     <row r="30">
@@ -2265,7 +2265,7 @@
         </is>
       </c>
       <c r="B30">
-        <v>-0.4867590281308179</v>
+        <v>-0.4867369095720636</v>
       </c>
     </row>
     <row r="31">
@@ -2275,7 +2275,7 @@
         </is>
       </c>
       <c r="B31">
-        <v>-0.7602244430399617</v>
+        <v>-0.7602845967965965</v>
       </c>
     </row>
     <row r="32">
@@ -2285,7 +2285,7 @@
         </is>
       </c>
       <c r="B32">
-        <v>0.3595955281148215</v>
+        <v>0.359603483035738</v>
       </c>
     </row>
     <row r="33">
@@ -2295,7 +2295,7 @@
         </is>
       </c>
       <c r="B33">
-        <v>0.3459442980078744</v>
+        <v>0.3459019826334064</v>
       </c>
     </row>
     <row r="34">
@@ -2305,7 +2305,7 @@
         </is>
       </c>
       <c r="B34">
-        <v>0.4060798370291895</v>
+        <v>0.4061285565244701</v>
       </c>
     </row>
     <row r="35">
@@ -2315,7 +2315,7 @@
         </is>
       </c>
       <c r="B35">
-        <v>0.5045114328102054</v>
+        <v>0.5045457816776494</v>
       </c>
     </row>
     <row r="36">
@@ -2325,7 +2325,7 @@
         </is>
       </c>
       <c r="B36">
-        <v>-0.48153691324385</v>
+        <v>-0.481524248697351</v>
       </c>
     </row>
     <row r="37">
@@ -2335,7 +2335,7 @@
         </is>
       </c>
       <c r="B37">
-        <v>0.2950518283772093</v>
+        <v>0.2950548429689773</v>
       </c>
     </row>
     <row r="38">
@@ -2345,7 +2345,7 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.2573424107862435</v>
+        <v>0.2573706138852802</v>
       </c>
     </row>
     <row r="39">
@@ -2355,7 +2355,7 @@
         </is>
       </c>
       <c r="B39">
-        <v>0.3184962041549603</v>
+        <v>0.3184657711645538</v>
       </c>
     </row>
     <row r="40">
@@ -2365,7 +2365,7 @@
         </is>
       </c>
       <c r="B40">
-        <v>0.4053564125483036</v>
+        <v>0.4053551458226133</v>
       </c>
     </row>
     <row r="41">
@@ -2375,7 +2375,7 @@
         </is>
       </c>
       <c r="B41">
-        <v>-0.908487768538303</v>
+        <v>-0.9085499374159322</v>
       </c>
     </row>
     <row r="42">
@@ -2385,7 +2385,7 @@
         </is>
       </c>
       <c r="B42">
-        <v>-0.5029640004576005</v>
+        <v>-0.5029264053670435</v>
       </c>
     </row>
     <row r="43">
@@ -2395,7 +2395,7 @@
         </is>
       </c>
       <c r="B43">
-        <v>-0.6192476795711415</v>
+        <v>-0.6192459781403306</v>
       </c>
     </row>
     <row r="44">
@@ -2405,7 +2405,7 @@
         </is>
       </c>
       <c r="B44">
-        <v>0.1082505079294222</v>
+        <v>0.108254071458422</v>
       </c>
     </row>
     <row r="45">
@@ -2415,7 +2415,7 @@
         </is>
       </c>
       <c r="B45">
-        <v>-0.9061900250460329</v>
+        <v>-0.9061440821427377</v>
       </c>
     </row>
     <row r="46">
@@ -2425,7 +2425,7 @@
         </is>
       </c>
       <c r="B46">
-        <v>0.3839226741093791</v>
+        <v>0.3838840067771572</v>
       </c>
     </row>
     <row r="47">
@@ -2435,7 +2435,7 @@
         </is>
       </c>
       <c r="B47">
-        <v>-0.9989533307713935</v>
+        <v>-0.9990091076818549</v>
       </c>
     </row>
     <row r="48">
@@ -2445,7 +2445,7 @@
         </is>
       </c>
       <c r="B48">
-        <v>-0.1192119463144712</v>
+        <v>-0.1191712240185101</v>
       </c>
     </row>
     <row r="49">
@@ -2455,7 +2455,7 @@
         </is>
       </c>
       <c r="B49">
-        <v>0.6349841239975005</v>
+        <v>0.6349998297246485</v>
       </c>
     </row>
     <row r="50">
@@ -2465,7 +2465,7 @@
         </is>
       </c>
       <c r="B50">
-        <v>-0.181134399411483</v>
+        <v>-0.1811750281739277</v>
       </c>
     </row>
     <row r="51">
@@ -2475,7 +2475,7 @@
         </is>
       </c>
       <c r="B51">
-        <v>0.3480684250318449</v>
+        <v>0.3480511155226464</v>
       </c>
     </row>
     <row r="52">
@@ -2485,7 +2485,7 @@
         </is>
       </c>
       <c r="B52">
-        <v>-0.7156133568765221</v>
+        <v>-0.715624447113231</v>
       </c>
     </row>
   </sheetData>
@@ -2535,16 +2535,16 @@
         </is>
       </c>
       <c r="B2">
-        <v>-1.552853273901155</v>
+        <v>-1.552975796082729</v>
       </c>
       <c r="C2">
-        <v>-1.319792966862148</v>
+        <v>-1.32034984627818</v>
       </c>
       <c r="D2">
-        <v>-1.338682609055229</v>
+        <v>-1.339763990857971</v>
       </c>
       <c r="E2">
-        <v>-1.383185946063802</v>
+        <v>-1.383089473562751</v>
       </c>
     </row>
     <row r="3">
@@ -2554,16 +2554,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>-0.8431620289226631</v>
+        <v>-0.8432506092089281</v>
       </c>
       <c r="C3">
-        <v>-1.161533488466614</v>
+        <v>-1.161309031842669</v>
       </c>
       <c r="D3">
-        <v>-1.519099084724192</v>
+        <v>-1.519294377745518</v>
       </c>
       <c r="E3">
-        <v>-1.139311714324985</v>
+        <v>-1.139305797550153</v>
       </c>
     </row>
     <row r="4">
@@ -2573,16 +2573,16 @@
         </is>
       </c>
       <c r="B4">
-        <v>-1.761740799382168</v>
+        <v>-1.761734223143563</v>
       </c>
       <c r="C4">
-        <v>-0.5659264718363847</v>
+        <v>-0.5653844387089546</v>
       </c>
       <c r="D4">
-        <v>-1.390155986736243</v>
+        <v>-1.390630204353133</v>
       </c>
       <c r="E4">
-        <v>-0.9989533307713935</v>
+        <v>-0.9990091076818549</v>
       </c>
     </row>
     <row r="5">
@@ -2592,16 +2592,16 @@
         </is>
       </c>
       <c r="B5">
-        <v>-1.033410100280771</v>
+        <v>-1.033491399908844</v>
       </c>
       <c r="C5">
-        <v>-0.7278781221028975</v>
+        <v>-0.7274778030566553</v>
       </c>
       <c r="D5">
-        <v>-0.9996755437711566</v>
+        <v>-1.000157506213422</v>
       </c>
       <c r="E5">
-        <v>-0.908487768538303</v>
+        <v>-0.9085499374159322</v>
       </c>
     </row>
     <row r="6">
@@ -2611,16 +2611,16 @@
         </is>
       </c>
       <c r="B6">
-        <v>-0.7195718048211917</v>
+        <v>-0.7195048374358026</v>
       </c>
       <c r="C6">
-        <v>-0.8972086450442145</v>
+        <v>-0.8966419594099232</v>
       </c>
       <c r="D6">
-        <v>-1.147967674508756</v>
+        <v>-1.147621739947163</v>
       </c>
       <c r="E6">
-        <v>-0.9061900250460329</v>
+        <v>-0.9061440821427377</v>
       </c>
     </row>
     <row r="7">
@@ -2630,16 +2630,16 @@
         </is>
       </c>
       <c r="B7">
-        <v>-0.4871918559230149</v>
+        <v>-0.4872098142395328</v>
       </c>
       <c r="C7">
-        <v>-0.7291918356475732</v>
+        <v>-0.7285725145158102</v>
       </c>
       <c r="D7">
-        <v>-1.817373075827484</v>
+        <v>-1.817570364420324</v>
       </c>
       <c r="E7">
-        <v>-0.7602244430399617</v>
+        <v>-0.7602845967965965</v>
       </c>
     </row>
     <row r="8">
@@ -2649,16 +2649,16 @@
         </is>
       </c>
       <c r="B8">
-        <v>-1.117523565389231</v>
+        <v>-1.117332931268181</v>
       </c>
       <c r="C8">
-        <v>-0.1848971421706865</v>
+        <v>-0.184778668832089</v>
       </c>
       <c r="D8">
-        <v>-0.7151345219911827</v>
+        <v>-0.7148687644027398</v>
       </c>
       <c r="E8">
-        <v>-0.7268839675391212</v>
+        <v>-0.7267822032957377</v>
       </c>
     </row>
     <row r="9">
@@ -2668,16 +2668,16 @@
         </is>
       </c>
       <c r="B9">
-        <v>-1.181768699621209</v>
+        <v>-1.181753096155747</v>
       </c>
       <c r="C9">
-        <v>-0.5973483075860188</v>
+        <v>-0.59612692302143</v>
       </c>
       <c r="D9">
-        <v>-0.287122638289798</v>
+        <v>-0.2858026104857197</v>
       </c>
       <c r="E9">
-        <v>-0.7156133568765221</v>
+        <v>-0.715624447113231</v>
       </c>
     </row>
     <row r="10">
@@ -2687,16 +2687,16 @@
         </is>
       </c>
       <c r="B10">
-        <v>-1.035912555809179</v>
+        <v>-1.035932860804692</v>
       </c>
       <c r="C10">
-        <v>-0.6643985931450389</v>
+        <v>-0.6635114185639509</v>
       </c>
       <c r="D10">
-        <v>0.2878917748667326</v>
+        <v>0.2887426042905565</v>
       </c>
       <c r="E10">
-        <v>-0.6192476795711415</v>
+        <v>-0.6192459781403306</v>
       </c>
     </row>
     <row r="11">
@@ -2706,16 +2706,16 @@
         </is>
       </c>
       <c r="B11">
-        <v>-0.6689488367979073</v>
+        <v>-0.6689075631707138</v>
       </c>
       <c r="C11">
-        <v>-0.4916521491586364</v>
+        <v>-0.4908425707899471</v>
       </c>
       <c r="D11">
-        <v>0.1603559275861986</v>
+        <v>0.1609906495855439</v>
       </c>
       <c r="E11">
-        <v>-0.5030986966213974</v>
+        <v>-0.5031087316277191</v>
       </c>
     </row>
     <row r="12">
@@ -2725,16 +2725,16 @@
         </is>
       </c>
       <c r="B12">
-        <v>-0.478316911800977</v>
+        <v>-0.4783282906657406</v>
       </c>
       <c r="C12">
-        <v>-0.9070795660533716</v>
+        <v>-0.9069177070273359</v>
       </c>
       <c r="D12">
-        <v>0.9436093807949301</v>
+        <v>0.9439845472270046</v>
       </c>
       <c r="E12">
-        <v>-0.5029640004576005</v>
+        <v>-0.5029264053670435</v>
       </c>
     </row>
     <row r="13">
@@ -2744,16 +2744,16 @@
         </is>
       </c>
       <c r="B13">
-        <v>-0.2838598611087938</v>
+        <v>-0.2838724847735811</v>
       </c>
       <c r="C13">
-        <v>-0.5341319504163035</v>
+        <v>-0.5332636949767861</v>
       </c>
       <c r="D13">
-        <v>-0.520275080862278</v>
+        <v>-0.5189931991410623</v>
       </c>
       <c r="E13">
-        <v>-0.4867590281308179</v>
+        <v>-0.4867369095720636</v>
       </c>
     </row>
     <row r="14">
@@ -2763,16 +2763,16 @@
         </is>
       </c>
       <c r="B14">
-        <v>0.07717723264610546</v>
+        <v>0.07722228031321896</v>
       </c>
       <c r="C14">
-        <v>-1.067881041730398</v>
+        <v>-1.066754424716891</v>
       </c>
       <c r="D14">
-        <v>0.093398188376644</v>
+        <v>0.09494033231427727</v>
       </c>
       <c r="E14">
-        <v>-0.48153691324385</v>
+        <v>-0.481524248697351</v>
       </c>
     </row>
     <row r="15">
@@ -2782,16 +2782,16 @@
         </is>
       </c>
       <c r="B15">
-        <v>-0.4572652922786732</v>
+        <v>-0.4573060797737802</v>
       </c>
       <c r="C15">
-        <v>-0.5574259748895422</v>
+        <v>-0.5573113811559901</v>
       </c>
       <c r="D15">
-        <v>0.6063989905054424</v>
+        <v>0.6071613831168229</v>
       </c>
       <c r="E15">
-        <v>-0.3977753829373302</v>
+        <v>-0.3977028980126575</v>
       </c>
     </row>
     <row r="16">
@@ -2801,16 +2801,16 @@
         </is>
       </c>
       <c r="B16">
-        <v>-0.2107096300663047</v>
+        <v>-0.2107326532823305</v>
       </c>
       <c r="C16">
-        <v>-0.1695175496852171</v>
+        <v>-0.1693193676389557</v>
       </c>
       <c r="D16">
-        <v>-0.08108460132415919</v>
+        <v>-0.08052430516249021</v>
       </c>
       <c r="E16">
-        <v>-0.3020155664608553</v>
+        <v>-0.3019866373008651</v>
       </c>
     </row>
     <row r="17">
@@ -2820,16 +2820,16 @@
         </is>
       </c>
       <c r="B17">
-        <v>-0.6481010370827559</v>
+        <v>-0.6480714110313354</v>
       </c>
       <c r="C17">
-        <v>0.1529810290138089</v>
+        <v>0.1538073161694786</v>
       </c>
       <c r="D17">
-        <v>-0.3961913442196406</v>
+        <v>-0.3958691021105883</v>
       </c>
       <c r="E17">
-        <v>-0.181134399411483</v>
+        <v>-0.1811750281739277</v>
       </c>
     </row>
     <row r="18">
@@ -2839,16 +2839,16 @@
         </is>
       </c>
       <c r="B18">
-        <v>-0.5567967572394513</v>
+        <v>-0.5567702826317268</v>
       </c>
       <c r="C18">
-        <v>0.2162570096603093</v>
+        <v>0.2167936097345974</v>
       </c>
       <c r="D18">
-        <v>-0.7748328378808831</v>
+        <v>-0.7743402444207682</v>
       </c>
       <c r="E18">
-        <v>-0.1579592759084945</v>
+        <v>-0.1579557983582583</v>
       </c>
     </row>
     <row r="19">
@@ -2858,16 +2858,16 @@
         </is>
       </c>
       <c r="B19">
-        <v>-0.1257070197089596</v>
+        <v>-0.1257026993871829</v>
       </c>
       <c r="C19">
-        <v>-0.8170496131347321</v>
+        <v>-0.8167676718071686</v>
       </c>
       <c r="D19">
-        <v>1.501961456250036</v>
+        <v>1.502668955877126</v>
       </c>
       <c r="E19">
-        <v>-0.1192119463144712</v>
+        <v>-0.1191712240185101</v>
       </c>
     </row>
     <row r="20">
@@ -2877,16 +2877,16 @@
         </is>
       </c>
       <c r="B20">
-        <v>0.4854471346242175</v>
+        <v>0.4854550930935883</v>
       </c>
       <c r="C20">
-        <v>-0.7158329774234646</v>
+        <v>-0.715674738110565</v>
       </c>
       <c r="D20">
-        <v>0.908533979818997</v>
+        <v>0.9090221850191205</v>
       </c>
       <c r="E20">
-        <v>-0.08180422970961104</v>
+        <v>-0.08173143486957839</v>
       </c>
     </row>
     <row r="21">
@@ -2896,16 +2896,16 @@
         </is>
       </c>
       <c r="B21">
-        <v>-0.4553647393943374</v>
+        <v>-0.455391379997536</v>
       </c>
       <c r="C21">
-        <v>0.1329313817510104</v>
+        <v>0.1337543727706917</v>
       </c>
       <c r="D21">
-        <v>0.5129763907551531</v>
+        <v>0.5135818556552071</v>
       </c>
       <c r="E21">
-        <v>-0.07609532274231182</v>
+        <v>-0.07613314752392485</v>
       </c>
     </row>
     <row r="22">
@@ -2915,16 +2915,16 @@
         </is>
       </c>
       <c r="B22">
-        <v>-0.3285805487383965</v>
+        <v>-0.3285089167286134</v>
       </c>
       <c r="C22">
-        <v>-0.2222181934628645</v>
+        <v>-0.221258738098225</v>
       </c>
       <c r="D22">
-        <v>-0.001742240811412345</v>
+        <v>8.38897759084388E-05</v>
       </c>
       <c r="E22">
-        <v>-0.05117455808853861</v>
+        <v>-0.05103854888699403</v>
       </c>
     </row>
     <row r="23">
@@ -2934,16 +2934,16 @@
         </is>
       </c>
       <c r="B23">
-        <v>0.9691686055704397</v>
+        <v>0.9691932892602967</v>
       </c>
       <c r="C23">
-        <v>-1.55549496684002</v>
+        <v>-1.554439630692183</v>
       </c>
       <c r="D23">
-        <v>-0.1008509340782001</v>
+        <v>-0.099980202326338</v>
       </c>
       <c r="E23">
-        <v>-0.0333722829406122</v>
+        <v>-0.03341395504256857</v>
       </c>
     </row>
     <row r="24">
@@ -2953,16 +2953,16 @@
         </is>
       </c>
       <c r="B24">
-        <v>0.3794926309675766</v>
+        <v>0.3795097030527969</v>
       </c>
       <c r="C24">
-        <v>0.01455118467319229</v>
+        <v>0.01489364812551331</v>
       </c>
       <c r="D24">
-        <v>-0.6659244183420761</v>
+        <v>-0.6658244192043324</v>
       </c>
       <c r="E24">
-        <v>0.04671982713181191</v>
+        <v>0.04674265139039078</v>
       </c>
     </row>
     <row r="25">
@@ -2972,16 +2972,16 @@
         </is>
       </c>
       <c r="B25">
-        <v>-0.5612322195000994</v>
+        <v>-0.5611821251704674</v>
       </c>
       <c r="C25">
-        <v>0.6007617578596708</v>
+        <v>0.6015464471938033</v>
       </c>
       <c r="D25">
-        <v>-0.4058869669265243</v>
+        <v>-0.4054127493802704</v>
       </c>
       <c r="E25">
-        <v>0.06604062630455311</v>
+        <v>0.06600286887826992</v>
       </c>
     </row>
     <row r="26">
@@ -2991,16 +2991,16 @@
         </is>
       </c>
       <c r="B26">
-        <v>0.7660564712056283</v>
+        <v>0.7660564747966165</v>
       </c>
       <c r="C26">
-        <v>-0.5668689407237995</v>
+        <v>-0.5668264315376936</v>
       </c>
       <c r="D26">
-        <v>0.8008471132227915</v>
+        <v>0.8014842078003478</v>
       </c>
       <c r="E26">
-        <v>0.09356018428129514</v>
+        <v>0.09363775263897317</v>
       </c>
     </row>
     <row r="27">
@@ -3010,16 +3010,16 @@
         </is>
       </c>
       <c r="B27">
-        <v>0.1928526531182913</v>
+        <v>0.1928727562928887</v>
       </c>
       <c r="C27">
-        <v>0.3711187768032389</v>
+        <v>0.3714712449322368</v>
       </c>
       <c r="D27">
-        <v>-1.092176983400562</v>
+        <v>-1.091923303097379</v>
       </c>
       <c r="E27">
-        <v>0.1082505079294222</v>
+        <v>0.108254071458422</v>
       </c>
     </row>
     <row r="28">
@@ -3029,16 +3029,16 @@
         </is>
       </c>
       <c r="B28">
-        <v>0.2968937320605084</v>
+        <v>0.296888637459287</v>
       </c>
       <c r="C28">
-        <v>0.2582801590122458</v>
+        <v>0.2590759701860573</v>
       </c>
       <c r="D28">
-        <v>0.6250417932104905</v>
+        <v>0.6258901529127305</v>
       </c>
       <c r="E28">
-        <v>0.2054379455306424</v>
+        <v>0.2054114404958935</v>
       </c>
     </row>
     <row r="29">
@@ -3048,16 +3048,16 @@
         </is>
       </c>
       <c r="B29">
-        <v>0.2246042860006618</v>
+        <v>0.2245907131098721</v>
       </c>
       <c r="C29">
-        <v>0.1456659546845397</v>
+        <v>0.1462103210071088</v>
       </c>
       <c r="D29">
-        <v>0.9693715148120021</v>
+        <v>0.9700139501012744</v>
       </c>
       <c r="E29">
-        <v>0.2573424107862435</v>
+        <v>0.2573706138852802</v>
       </c>
     </row>
     <row r="30">
@@ -3067,16 +3067,16 @@
         </is>
       </c>
       <c r="B30">
-        <v>-0.08597802141424034</v>
+        <v>-0.08596922480107251</v>
       </c>
       <c r="C30">
-        <v>0.7824550971442956</v>
+        <v>0.7823505612690713</v>
       </c>
       <c r="D30">
-        <v>-1.325354520439601</v>
+        <v>-1.322635601011907</v>
       </c>
       <c r="E30">
-        <v>0.2769068821245325</v>
+        <v>0.277147421522158</v>
       </c>
     </row>
     <row r="31">
@@ -3086,16 +3086,16 @@
         </is>
       </c>
       <c r="B31">
-        <v>0.006859567148981245</v>
+        <v>0.006862388379346735</v>
       </c>
       <c r="C31">
-        <v>0.6529964460021935</v>
+        <v>0.6534530988280282</v>
       </c>
       <c r="D31">
-        <v>-0.3381124835335337</v>
+        <v>-0.3378632060941346</v>
       </c>
       <c r="E31">
-        <v>0.2848382100113157</v>
+        <v>0.2848261746449285</v>
       </c>
     </row>
     <row r="32">
@@ -3105,16 +3105,16 @@
         </is>
       </c>
       <c r="B32">
-        <v>-0.4142333487413991</v>
+        <v>-0.4141713454091082</v>
       </c>
       <c r="C32">
-        <v>0.8280519601031143</v>
+        <v>0.8283593738336013</v>
       </c>
       <c r="D32">
-        <v>0.2719570392224911</v>
+        <v>0.2719948792944492</v>
       </c>
       <c r="E32">
-        <v>0.2950518283772093</v>
+        <v>0.2950548429689773</v>
       </c>
     </row>
     <row r="33">
@@ -3124,16 +3124,16 @@
         </is>
       </c>
       <c r="B33">
-        <v>-1.115999566352717</v>
+        <v>-1.11604088344161</v>
       </c>
       <c r="C33">
-        <v>0.7732870878610397</v>
+        <v>0.7736869647904464</v>
       </c>
       <c r="D33">
-        <v>0.189179946740731</v>
+        <v>0.1885960941099055</v>
       </c>
       <c r="E33">
-        <v>0.2996678411792817</v>
+        <v>0.2996367603965951</v>
       </c>
     </row>
     <row r="34">
@@ -3143,16 +3143,16 @@
         </is>
       </c>
       <c r="B34">
-        <v>0.2471326585944414</v>
+        <v>0.2471596654245625</v>
       </c>
       <c r="C34">
-        <v>0.3993001077312155</v>
+        <v>0.3998274485635739</v>
       </c>
       <c r="D34">
-        <v>0.8780827567853325</v>
+        <v>0.8780532986105821</v>
       </c>
       <c r="E34">
-        <v>0.3184962041549603</v>
+        <v>0.3184657711645538</v>
       </c>
     </row>
     <row r="35">
@@ -3162,16 +3162,16 @@
         </is>
       </c>
       <c r="B35">
-        <v>0.506367630133558</v>
+        <v>0.5063278499450848</v>
       </c>
       <c r="C35">
-        <v>0.05089073959906423</v>
+        <v>0.051915315694388</v>
       </c>
       <c r="D35">
-        <v>0.6969433915405137</v>
+        <v>0.6970216174240549</v>
       </c>
       <c r="E35">
-        <v>0.3459442980078744</v>
+        <v>0.3459019826334064</v>
       </c>
     </row>
     <row r="36">
@@ -3181,16 +3181,16 @@
         </is>
       </c>
       <c r="B36">
-        <v>0.4734040413373887</v>
+        <v>0.4734487870484301</v>
       </c>
       <c r="C36">
-        <v>0.2677114387654328</v>
+        <v>0.2683362390492197</v>
       </c>
       <c r="D36">
-        <v>1.212004862982891</v>
+        <v>1.212431872265201</v>
       </c>
       <c r="E36">
-        <v>0.3480684250318449</v>
+        <v>0.3480511155226464</v>
       </c>
     </row>
     <row r="37">
@@ -3200,16 +3200,16 @@
         </is>
       </c>
       <c r="B37">
-        <v>0.5622937104604721</v>
+        <v>0.5622308029564578</v>
       </c>
       <c r="C37">
-        <v>0.390212056931589</v>
+        <v>0.3905794781572773</v>
       </c>
       <c r="D37">
-        <v>-0.03176435963002326</v>
+        <v>-0.03162857461862049</v>
       </c>
       <c r="E37">
-        <v>0.3595955281148215</v>
+        <v>0.359603483035738</v>
       </c>
     </row>
     <row r="38">
@@ -3219,16 +3219,16 @@
         </is>
       </c>
       <c r="B38">
-        <v>0.981367213570524</v>
+        <v>0.9814045632970432</v>
       </c>
       <c r="C38">
-        <v>-0.1644564990618951</v>
+        <v>-0.1634361948990848</v>
       </c>
       <c r="D38">
-        <v>0.5756421516157544</v>
+        <v>0.5768793844482697</v>
       </c>
       <c r="E38">
-        <v>0.3839226741093791</v>
+        <v>0.3838840067771572</v>
       </c>
     </row>
     <row r="39">
@@ -3238,16 +3238,16 @@
         </is>
       </c>
       <c r="B39">
-        <v>0.523488094696101</v>
+        <v>0.5235084108411926</v>
       </c>
       <c r="C39">
-        <v>0.6086614245791945</v>
+        <v>0.6091990020524504</v>
       </c>
       <c r="D39">
-        <v>-0.383059343662972</v>
+        <v>-0.3827834487002213</v>
       </c>
       <c r="E39">
-        <v>0.4029436908643569</v>
+        <v>0.4029260464877222</v>
       </c>
     </row>
     <row r="40">
@@ -3257,16 +3257,16 @@
         </is>
       </c>
       <c r="B40">
-        <v>0.4930437594810862</v>
+        <v>0.4930834592983986</v>
       </c>
       <c r="C40">
-        <v>0.6592785062088932</v>
+        <v>0.6595979467188182</v>
       </c>
       <c r="D40">
-        <v>-0.7527965231078599</v>
+        <v>-0.7528404639440259</v>
       </c>
       <c r="E40">
-        <v>0.4053564125483036</v>
+        <v>0.4053551458226133</v>
       </c>
     </row>
     <row r="41">
@@ -3276,16 +3276,16 @@
         </is>
       </c>
       <c r="B41">
-        <v>-0.4878818198784703</v>
+        <v>-0.4878658938491042</v>
       </c>
       <c r="C41">
-        <v>0.8836500175751054</v>
+        <v>0.8836475993565989</v>
       </c>
       <c r="D41">
-        <v>0.9770345967824766</v>
+        <v>0.9766506366266791</v>
       </c>
       <c r="E41">
-        <v>0.4060798370291895</v>
+        <v>0.4061285565244701</v>
       </c>
     </row>
     <row r="42">
@@ -3295,16 +3295,16 @@
         </is>
       </c>
       <c r="B42">
-        <v>0.9145510847677037</v>
+        <v>0.9145218025375009</v>
       </c>
       <c r="C42">
-        <v>0.1730345095767379</v>
+        <v>0.1736367345547335</v>
       </c>
       <c r="D42">
-        <v>-0.09616480938771775</v>
+        <v>-0.09636425964788412</v>
       </c>
       <c r="E42">
-        <v>0.406945892534713</v>
+        <v>0.4068774618731519</v>
       </c>
     </row>
     <row r="43">
@@ -3314,16 +3314,16 @@
         </is>
       </c>
       <c r="B43">
-        <v>1.065249799183251</v>
+        <v>1.065256617684329</v>
       </c>
       <c r="C43">
-        <v>0.2846845287788118</v>
+        <v>0.284861343224673</v>
       </c>
       <c r="D43">
-        <v>0.3624579894666846</v>
+        <v>0.3629004436065341</v>
       </c>
       <c r="E43">
-        <v>0.5045114328102054</v>
+        <v>0.5045457816776494</v>
       </c>
     </row>
     <row r="44">
@@ -3333,16 +3333,16 @@
         </is>
       </c>
       <c r="B44">
-        <v>0.5665803266537462</v>
+        <v>0.566637787777987</v>
       </c>
       <c r="C44">
-        <v>0.6668616651813118</v>
+        <v>0.6671970054292965</v>
       </c>
       <c r="D44">
-        <v>0.9495624392872207</v>
+        <v>0.9500224040172693</v>
       </c>
       <c r="E44">
-        <v>0.5077498607958199</v>
+        <v>0.5077635258330078</v>
       </c>
     </row>
     <row r="45">
@@ -3352,16 +3352,16 @@
         </is>
       </c>
       <c r="B45">
-        <v>0.08499270357886061</v>
+        <v>0.08494002554866097</v>
       </c>
       <c r="C45">
-        <v>0.8927563695169739</v>
+        <v>0.892973869840605</v>
       </c>
       <c r="D45">
-        <v>0.1130276854167859</v>
+        <v>0.1123345316256893</v>
       </c>
       <c r="E45">
-        <v>0.513599965829839</v>
+        <v>0.5135632486058881</v>
       </c>
     </row>
     <row r="46">
@@ -3371,16 +3371,16 @@
         </is>
       </c>
       <c r="B46">
-        <v>1.162128347750292</v>
+        <v>1.162077842411568</v>
       </c>
       <c r="C46">
-        <v>0.2316367538777333</v>
+        <v>0.2315727400495358</v>
       </c>
       <c r="D46">
-        <v>1.145267821326315</v>
+        <v>1.145441762336221</v>
       </c>
       <c r="E46">
-        <v>0.6256512355291427</v>
+        <v>0.6257066645208705</v>
       </c>
     </row>
     <row r="47">
@@ -3390,16 +3390,16 @@
         </is>
       </c>
       <c r="B47">
-        <v>0.8626092557968615</v>
+        <v>0.8626238570950225</v>
       </c>
       <c r="C47">
-        <v>0.653328510049679</v>
+        <v>0.6541278080871633</v>
       </c>
       <c r="D47">
-        <v>0.2768029718096486</v>
+        <v>0.2772329702369824</v>
       </c>
       <c r="E47">
-        <v>0.6310724272858534</v>
+        <v>0.6310530559667228</v>
       </c>
     </row>
     <row r="48">
@@ -3409,16 +3409,16 @@
         </is>
       </c>
       <c r="B48">
-        <v>0.8419302401053328</v>
+        <v>0.8420100714767016</v>
       </c>
       <c r="C48">
-        <v>0.6075191316218623</v>
+        <v>0.6080610976246914</v>
       </c>
       <c r="D48">
-        <v>1.082816743681575</v>
+        <v>1.083485450638274</v>
       </c>
       <c r="E48">
-        <v>0.6349841239975005</v>
+        <v>0.6349998297246485</v>
       </c>
     </row>
     <row r="49">
@@ -3428,16 +3428,16 @@
         </is>
       </c>
       <c r="B49">
-        <v>0.8800417775141355</v>
+        <v>0.8800893255643465</v>
       </c>
       <c r="C49">
-        <v>0.6105811503632724</v>
+        <v>0.6112430370159492</v>
       </c>
       <c r="D49">
-        <v>1.045435267274211</v>
+        <v>1.046011821030861</v>
       </c>
       <c r="E49">
-        <v>0.6352508032987695</v>
+        <v>0.6352388679954268</v>
       </c>
     </row>
     <row r="50">
@@ -3447,16 +3447,16 @@
         </is>
       </c>
       <c r="B50">
-        <v>0.7868800587357219</v>
+        <v>0.7869228202624792</v>
       </c>
       <c r="C50">
-        <v>0.8892840879685002</v>
+        <v>0.889625582256208</v>
       </c>
       <c r="D50">
-        <v>0.01635656530065821</v>
+        <v>0.01654093906740731</v>
       </c>
       <c r="E50">
-        <v>0.6654125039776517</v>
+        <v>0.6654307875349142</v>
       </c>
     </row>
     <row r="51">
@@ -3466,16 +3466,16 @@
         </is>
       </c>
       <c r="B51">
-        <v>1.183302178448496</v>
+        <v>1.183351418893715</v>
       </c>
       <c r="C51">
-        <v>0.6253208964046587</v>
+        <v>0.6260223068331543</v>
       </c>
       <c r="D51">
-        <v>0.05854339432051642</v>
+        <v>0.05902901130349057</v>
       </c>
       <c r="E51">
-        <v>0.7349134033300365</v>
+        <v>0.7348930505083187</v>
       </c>
     </row>
     <row r="52">
@@ -3485,16 +3485,16 @@
         </is>
       </c>
       <c r="B52">
-        <v>1.213808316179295</v>
+        <v>1.213865710618471</v>
       </c>
       <c r="C52">
-        <v>0.8608567444383043</v>
+        <v>0.8614730259207737</v>
       </c>
       <c r="D52">
-        <v>-0.6447373117067832</v>
+        <v>-0.6443361590093264</v>
       </c>
       <c r="E52">
-        <v>0.8026895054318718</v>
+        <v>0.8026651320446875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>